<commit_message>
Cleaned Code and made it prettier
</commit_message>
<xml_diff>
--- a/Bauteileschrank.xlsx
+++ b/Bauteileschrank.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,7 +520,7 @@
         <v>10000004</v>
       </c>
       <c r="B6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -534,7 +534,7 @@
         <v>10000005</v>
       </c>
       <c r="B7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -548,7 +548,7 @@
         <v>10000006</v>
       </c>
       <c r="B8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
         <v>10000007</v>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -576,7 +576,7 @@
         <v>10000008</v>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -590,7 +590,7 @@
         <v>10000009</v>
       </c>
       <c r="B11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -604,7 +604,7 @@
         <v>10000010</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -863,8 +863,10 @@
           <t>Some description</t>
         </is>
       </c>
-      <c r="D30" t="b">
-        <v>1</v>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -884,6 +886,46 @@
           <t>New Description</t>
         </is>
       </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>10000030</v>
+      </c>
+      <c r="B32" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>neues Teil</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>10000032</v>
+      </c>
+      <c r="B33" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>200</v>
+      </c>
+      <c r="D33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>10000031</v>
+      </c>
+      <c r="B34" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Teil 281</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   Bauteilemanager.py 	modified:   Bauteileschrank.xlsx
</commit_message>
<xml_diff>
--- a/Bauteileschrank.xlsx
+++ b/Bauteileschrank.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,7 +520,7 @@
         <v>10000004</v>
       </c>
       <c r="B6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -534,7 +534,7 @@
         <v>10000005</v>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -548,7 +548,7 @@
         <v>10000006</v>
       </c>
       <c r="B8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
         <v>10000007</v>
       </c>
       <c r="B9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -576,7 +576,7 @@
         <v>10000008</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -590,7 +590,7 @@
         <v>10000009</v>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -604,7 +604,7 @@
         <v>10000010</v>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -860,14 +860,10 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Some description</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
+          <t>Part 29</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -878,14 +874,10 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>New Part</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>New Description</t>
-        </is>
-      </c>
+          <t>Part 10xx</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -896,36 +888,24 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>neues Teil</t>
+          <t>art 10xx</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>10000032</v>
+        <v>10000031</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
       </c>
-      <c r="C33" t="n">
-        <v>200</v>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Oi</t>
+        </is>
       </c>
       <c r="D33" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>10000031</v>
-      </c>
-      <c r="B34" t="b">
-        <v>1</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Teil 281</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>